<commit_message>
working on graphics explainer
</commit_message>
<xml_diff>
--- a/election-night-graphics/data/election_night_master.xlsx
+++ b/election-night-graphics/data/election_night_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/election-night-app/election-night-graphics/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindsayhuth/Documents/GitHub/election-night-app/election-night-graphics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9664CBD6-C1B8-114D-AA66-CB2C4C79FB4C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8397BD38-B714-6447-A026-5ECAB2E693F3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22780" yWindow="1620" windowWidth="27240" windowHeight="25580" activeTab="3" xr2:uid="{EF519B7F-F581-D644-9218-2E498586D9F3}"/>
+    <workbookView xWindow="2480" yWindow="460" windowWidth="24680" windowHeight="16400" firstSheet="2" activeTab="8" xr2:uid="{EF519B7F-F581-D644-9218-2E498586D9F3}"/>
   </bookViews>
   <sheets>
     <sheet name="turnout-state" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,11 @@
     <sheet name="voting-county" sheetId="4" r:id="rId4"/>
     <sheet name="earlybycand" sheetId="5" r:id="rId5"/>
     <sheet name="mdrepoutcomes" sheetId="6" r:id="rId6"/>
+    <sheet name="graphic1" sheetId="7" r:id="rId7"/>
+    <sheet name="graphic2" sheetId="8" r:id="rId8"/>
+    <sheet name="graphic4" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="80">
   <si>
     <t>Year</t>
   </si>
@@ -244,16 +247,44 @@
   <si>
     <t>Pct chg early</t>
   </si>
+  <si>
+    <t>Hogan Votes 2014</t>
+  </si>
+  <si>
+    <t>Hogan Votes 2018</t>
+  </si>
+  <si>
+    <t>Pct Hogan 2014</t>
+  </si>
+  <si>
+    <t>Pct Hogan 2018</t>
+  </si>
+  <si>
+    <t>All Gov. Votes 2014</t>
+  </si>
+  <si>
+    <t>All Gov. Votes 2018</t>
+  </si>
+  <si>
+    <t>Pct Pt Diff</t>
+  </si>
+  <si>
+    <t>Pct Chg</t>
+  </si>
+  <si>
+    <t>Rep</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-10409]#,##0;\(#,##0\)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -371,7 +402,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
@@ -484,6 +515,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5936,8 +5969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA39EE2-8F56-3043-918D-52D7AD3C50B1}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6044,11 +6077,11 @@
         <v>20039</v>
       </c>
       <c r="E3" s="39">
-        <f>B3/SUM($B3:$C3)</f>
+        <f t="shared" ref="E3:E26" si="0">B3/SUM($B3:$C3)</f>
         <v>0.76900044912420784</v>
       </c>
       <c r="F3" s="35">
-        <f>C3/SUM($B3:$C3)</f>
+        <f t="shared" ref="F3:F26" si="1">C3/SUM($B3:$C3)</f>
         <v>0.23099955087579221</v>
       </c>
       <c r="G3" s="33">
@@ -6062,11 +6095,11 @@
         <v>21253</v>
       </c>
       <c r="J3" s="40">
-        <f>G3/SUM($G3:$H3)</f>
+        <f t="shared" ref="J3:J26" si="2">G3/SUM($G3:$H3)</f>
         <v>0.84919776031619065</v>
       </c>
       <c r="K3" s="36">
-        <f>H3/SUM($G3:$H3)</f>
+        <f t="shared" ref="K3:K26" si="3">H3/SUM($G3:$H3)</f>
         <v>0.15080223968380935</v>
       </c>
       <c r="L3" s="31">
@@ -6116,15 +6149,15 @@
         <v>58001</v>
       </c>
       <c r="D4" s="34">
-        <f t="shared" ref="D4:D26" si="0">SUM(B4:C4)</f>
+        <f t="shared" ref="D4:D26" si="4">SUM(B4:C4)</f>
         <v>177196</v>
       </c>
       <c r="E4" s="39">
-        <f>B4/SUM($B4:$C4)</f>
+        <f t="shared" si="0"/>
         <v>0.67267319804058778</v>
       </c>
       <c r="F4" s="35">
-        <f>C4/SUM($B4:$C4)</f>
+        <f t="shared" si="1"/>
         <v>0.32732680195941216</v>
       </c>
       <c r="G4" s="33">
@@ -6134,50 +6167,50 @@
         <v>63388</v>
       </c>
       <c r="I4" s="33">
-        <f t="shared" ref="I4:I26" si="1">SUM(G4:H4)</f>
+        <f t="shared" ref="I4:I26" si="5">SUM(G4:H4)</f>
         <v>211373</v>
       </c>
       <c r="J4" s="40">
-        <f>G4/SUM($G4:$H4)</f>
+        <f t="shared" si="2"/>
         <v>0.70011307025968317</v>
       </c>
       <c r="K4" s="36">
-        <f>H4/SUM($G4:$H4)</f>
+        <f t="shared" si="3"/>
         <v>0.29988692974031689</v>
       </c>
       <c r="L4" s="31">
-        <f t="shared" ref="L4:L26" si="2">G4-B4</f>
+        <f t="shared" ref="L4:L26" si="6">G4-B4</f>
         <v>28790</v>
       </c>
       <c r="M4" s="31">
-        <f t="shared" ref="M4:M26" si="3">H4-C4</f>
+        <f t="shared" ref="M4:M26" si="7">H4-C4</f>
         <v>5387</v>
       </c>
       <c r="N4" s="36">
-        <f t="shared" ref="N4:N26" si="4">(G4-B4)/B4</f>
+        <f t="shared" ref="N4:N26" si="8">(G4-B4)/B4</f>
         <v>0.24153697722219891</v>
       </c>
       <c r="O4" s="36">
-        <f t="shared" ref="O4:O26" si="5">(H4-C4)/C4</f>
+        <f t="shared" ref="O4:O26" si="9">(H4-C4)/C4</f>
         <v>9.2877709005017156E-2</v>
       </c>
       <c r="P4" s="4">
-        <f t="shared" ref="P4:P26" si="6">J4-E4</f>
+        <f t="shared" ref="P4:P26" si="10">J4-E4</f>
         <v>2.7439872219095385E-2</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q26" si="7">K4-F4</f>
+        <f t="shared" ref="Q4:Q26" si="11">K4-F4</f>
         <v>-2.7439872219095274E-2</v>
       </c>
       <c r="R4" s="36">
-        <f t="shared" ref="R4:R26" si="8">(I4-D4)/D4</f>
+        <f t="shared" ref="R4:R26" si="12">(I4-D4)/D4</f>
         <v>0.19287681437504234</v>
       </c>
       <c r="S4" s="31">
         <v>134806</v>
       </c>
       <c r="T4" s="31">
-        <f t="shared" ref="T4:T26" si="9">G4-S4</f>
+        <f t="shared" ref="T4:T26" si="13">G4-S4</f>
         <v>13179</v>
       </c>
     </row>
@@ -6192,15 +6225,15 @@
         <v>106213</v>
       </c>
       <c r="D5" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>137058</v>
       </c>
       <c r="E5" s="44">
-        <f>B5/SUM($B5:$C5)</f>
+        <f t="shared" si="0"/>
         <v>0.22505070845919245</v>
       </c>
       <c r="F5" s="44">
-        <f>C5/SUM($B5:$C5)</f>
+        <f t="shared" si="1"/>
         <v>0.77494929154080749</v>
       </c>
       <c r="G5" s="45">
@@ -6210,50 +6243,50 @@
         <v>113142</v>
       </c>
       <c r="I5" s="45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>167278</v>
       </c>
       <c r="J5" s="46">
-        <f>G5/SUM($G5:$H5)</f>
+        <f t="shared" si="2"/>
         <v>0.32362892908810481</v>
       </c>
       <c r="K5" s="46">
-        <f>H5/SUM($G5:$H5)</f>
+        <f t="shared" si="3"/>
         <v>0.67637107091189519</v>
       </c>
       <c r="L5" s="47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>23291</v>
       </c>
       <c r="M5" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6929</v>
       </c>
       <c r="N5" s="46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.75509807100016213</v>
       </c>
       <c r="O5" s="46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.5236835415627095E-2</v>
       </c>
       <c r="P5" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>9.8578220628912361E-2</v>
       </c>
       <c r="Q5" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-9.8578220628912305E-2</v>
       </c>
       <c r="R5" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.22049059522246056</v>
       </c>
       <c r="S5" s="47">
         <v>30873</v>
       </c>
       <c r="T5" s="47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>23263</v>
       </c>
     </row>
@@ -6268,15 +6301,15 @@
         <v>102734</v>
       </c>
       <c r="D6" s="55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>258670</v>
       </c>
       <c r="E6" s="39">
-        <f>B6/SUM($B6:$C6)</f>
+        <f t="shared" si="0"/>
         <v>0.6028375922990683</v>
       </c>
       <c r="F6" s="56">
-        <f>C6/SUM($B6:$C6)</f>
+        <f t="shared" si="1"/>
         <v>0.3971624077009317</v>
       </c>
       <c r="G6" s="57">
@@ -6286,50 +6319,50 @@
         <v>113565</v>
       </c>
       <c r="I6" s="57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>301675</v>
       </c>
       <c r="J6" s="40">
-        <f>G6/SUM($G6:$H6)</f>
+        <f t="shared" si="2"/>
         <v>0.62355183558465233</v>
       </c>
       <c r="K6" s="58">
-        <f>H6/SUM($G6:$H6)</f>
+        <f t="shared" si="3"/>
         <v>0.37644816441534762</v>
       </c>
       <c r="L6" s="59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32174</v>
       </c>
       <c r="M6" s="59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>10831</v>
       </c>
       <c r="N6" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.20632823722552843</v>
       </c>
       <c r="O6" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.10542760916541749</v>
       </c>
       <c r="P6" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.0714243285584022E-2</v>
       </c>
       <c r="Q6" s="60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-2.0714243285584077E-2</v>
       </c>
       <c r="R6" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.16625430084663859</v>
       </c>
       <c r="S6" s="59">
         <v>142739</v>
       </c>
       <c r="T6" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>45371</v>
       </c>
     </row>
@@ -6344,15 +6377,15 @@
         <v>9579</v>
       </c>
       <c r="D7" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>32318</v>
       </c>
       <c r="E7" s="39">
-        <f>B7/SUM($B7:$C7)</f>
+        <f t="shared" si="0"/>
         <v>0.70360170802648681</v>
       </c>
       <c r="F7" s="35">
-        <f>C7/SUM($B7:$C7)</f>
+        <f t="shared" si="1"/>
         <v>0.29639829197351319</v>
       </c>
       <c r="G7" s="33">
@@ -6362,50 +6395,50 @@
         <v>8452</v>
       </c>
       <c r="I7" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>36551</v>
       </c>
       <c r="J7" s="40">
-        <f>G7/SUM($G7:$H7)</f>
+        <f t="shared" si="2"/>
         <v>0.76876145659489481</v>
       </c>
       <c r="K7" s="36">
-        <f>H7/SUM($G7:$H7)</f>
+        <f t="shared" si="3"/>
         <v>0.23123854340510519</v>
       </c>
       <c r="L7" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5360</v>
       </c>
       <c r="M7" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1127</v>
       </c>
       <c r="N7" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.23571836932143014</v>
       </c>
       <c r="O7" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.11765319970769392</v>
       </c>
       <c r="P7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6.5159748568408005E-2</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-6.5159748568408005E-2</v>
       </c>
       <c r="R7" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.13097963982919736</v>
       </c>
       <c r="S7" s="31">
         <v>27415</v>
       </c>
       <c r="T7" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>684</v>
       </c>
     </row>
@@ -6420,15 +6453,15 @@
         <v>1931</v>
       </c>
       <c r="D8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9075</v>
       </c>
       <c r="E8" s="39">
-        <f>B8/SUM($B8:$C8)</f>
+        <f t="shared" si="0"/>
         <v>0.78721763085399454</v>
       </c>
       <c r="F8" s="35">
-        <f>C8/SUM($B8:$C8)</f>
+        <f t="shared" si="1"/>
         <v>0.21278236914600551</v>
       </c>
       <c r="G8" s="32">
@@ -6438,50 +6471,50 @@
         <v>1795</v>
       </c>
       <c r="I8" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>10961</v>
       </c>
       <c r="J8" s="40">
-        <f>G8/SUM($G8:$H8)</f>
+        <f t="shared" si="2"/>
         <v>0.83623756956482076</v>
       </c>
       <c r="K8" s="36">
-        <f>H8/SUM($G8:$H8)</f>
+        <f t="shared" si="3"/>
         <v>0.16376243043517927</v>
       </c>
       <c r="L8" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2022</v>
       </c>
       <c r="M8" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-136</v>
       </c>
       <c r="N8" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.28303471444568867</v>
       </c>
       <c r="O8" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-7.0429829104091138E-2</v>
       </c>
       <c r="P8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.9019938710826216E-2</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-4.9019938710826244E-2</v>
       </c>
       <c r="R8" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.20782369146005511</v>
       </c>
       <c r="S8" s="31">
         <v>9390</v>
       </c>
       <c r="T8" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-224</v>
       </c>
     </row>
@@ -6496,15 +6529,15 @@
         <v>10349</v>
       </c>
       <c r="D9" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63300</v>
       </c>
       <c r="E9" s="39">
-        <f>B9/SUM($B9:$C9)</f>
+        <f t="shared" si="0"/>
         <v>0.83650868878357032</v>
       </c>
       <c r="F9" s="35">
-        <f>C9/SUM($B9:$C9)</f>
+        <f t="shared" si="1"/>
         <v>0.16349131121642971</v>
       </c>
       <c r="G9" s="33">
@@ -6514,50 +6547,50 @@
         <v>10831</v>
       </c>
       <c r="I9" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>71045</v>
       </c>
       <c r="J9" s="40">
-        <f>G9/SUM($G9:$H9)</f>
+        <f t="shared" si="2"/>
         <v>0.84754732915757613</v>
       </c>
       <c r="K9" s="36">
-        <f>H9/SUM($G9:$H9)</f>
+        <f t="shared" si="3"/>
         <v>0.15245267084242381</v>
       </c>
       <c r="L9" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7263</v>
       </c>
       <c r="M9" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>482</v>
       </c>
       <c r="N9" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.13716454835602726</v>
       </c>
       <c r="O9" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.6574548265532902E-2</v>
       </c>
       <c r="P9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.1038640374005815E-2</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-1.1038640374005898E-2</v>
       </c>
       <c r="R9" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.12235387045813587</v>
       </c>
       <c r="S9" s="31">
         <v>62908</v>
       </c>
       <c r="T9" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-2694</v>
       </c>
     </row>
@@ -6572,15 +6605,15 @@
         <v>5467</v>
       </c>
       <c r="D10" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>26166</v>
       </c>
       <c r="E10" s="39">
-        <f>B10/SUM($B10:$C10)</f>
+        <f t="shared" si="0"/>
         <v>0.79106474050294273</v>
       </c>
       <c r="F10" s="35">
-        <f>C10/SUM($B10:$C10)</f>
+        <f t="shared" si="1"/>
         <v>0.20893525949705724</v>
       </c>
       <c r="G10" s="33">
@@ -6590,50 +6623,50 @@
         <v>6911</v>
       </c>
       <c r="I10" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>33082</v>
       </c>
       <c r="J10" s="40">
-        <f>G10/SUM($G10:$H10)</f>
+        <f t="shared" si="2"/>
         <v>0.79109485520827039</v>
       </c>
       <c r="K10" s="36">
-        <f>H10/SUM($G10:$H10)</f>
+        <f t="shared" si="3"/>
         <v>0.20890514479172964</v>
       </c>
       <c r="L10" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5472</v>
       </c>
       <c r="M10" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1444</v>
       </c>
       <c r="N10" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.26436059713029614</v>
       </c>
       <c r="O10" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.26413023596122187</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.0114705327655145E-5</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.0114705327599633E-5</v>
       </c>
       <c r="R10" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.26431246655965757</v>
       </c>
       <c r="S10" s="31">
         <v>28190</v>
       </c>
       <c r="T10" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-2019</v>
       </c>
     </row>
@@ -6648,15 +6681,15 @@
         <v>24601</v>
       </c>
       <c r="D11" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>46869</v>
       </c>
       <c r="E11" s="39">
-        <f>B11/SUM($B11:$C11)</f>
+        <f t="shared" si="0"/>
         <v>0.47511148093622652</v>
       </c>
       <c r="F11" s="35">
-        <f>C11/SUM($B11:$C11)</f>
+        <f t="shared" si="1"/>
         <v>0.52488851906377354</v>
       </c>
       <c r="G11" s="33">
@@ -6666,50 +6699,50 @@
         <v>30274</v>
       </c>
       <c r="I11" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>60568</v>
       </c>
       <c r="J11" s="40">
-        <f>G11/SUM($G11:$H11)</f>
+        <f t="shared" si="2"/>
         <v>0.50016510368511424</v>
       </c>
       <c r="K11" s="36">
-        <f>H11/SUM($G11:$H11)</f>
+        <f t="shared" si="3"/>
         <v>0.49983489631488576</v>
       </c>
       <c r="L11" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8026</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>5673</v>
       </c>
       <c r="N11" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.36042751931022093</v>
       </c>
       <c r="O11" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.23060038209828868</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.5053622748887727E-2</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-2.5053622748887783E-2</v>
       </c>
       <c r="R11" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.29228274552476052</v>
       </c>
       <c r="S11" s="31">
         <v>24871</v>
       </c>
       <c r="T11" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>5423</v>
       </c>
     </row>
@@ -6724,15 +6757,15 @@
         <v>3252</v>
       </c>
       <c r="D12" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10528</v>
       </c>
       <c r="E12" s="39">
-        <f>B12/SUM($B12:$C12)</f>
+        <f t="shared" si="0"/>
         <v>0.69110942249240126</v>
       </c>
       <c r="F12" s="35">
-        <f>C12/SUM($B12:$C12)</f>
+        <f t="shared" si="1"/>
         <v>0.3088905775075988</v>
       </c>
       <c r="G12" s="33">
@@ -6742,50 +6775,50 @@
         <v>2844</v>
       </c>
       <c r="I12" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>11565</v>
       </c>
       <c r="J12" s="40">
-        <f>G12/SUM($G12:$H12)</f>
+        <f t="shared" si="2"/>
         <v>0.75408560311284045</v>
       </c>
       <c r="K12" s="36">
-        <f>H12/SUM($G12:$H12)</f>
+        <f t="shared" si="3"/>
         <v>0.24591439688715952</v>
       </c>
       <c r="L12" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1445</v>
       </c>
       <c r="M12" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-408</v>
       </c>
       <c r="N12" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.19859813084112149</v>
       </c>
       <c r="O12" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.12546125461254612</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6.2976180620439193E-2</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-6.2976180620439276E-2</v>
       </c>
       <c r="R12" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9.8499240121580553E-2</v>
       </c>
       <c r="S12" s="31">
         <v>8182</v>
       </c>
       <c r="T12" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>539</v>
       </c>
     </row>
@@ -6800,15 +6833,15 @@
         <v>27682</v>
       </c>
       <c r="D13" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>78397</v>
       </c>
       <c r="E13" s="39">
-        <f>B13/SUM($B13:$C13)</f>
+        <f t="shared" si="0"/>
         <v>0.6468997538171104</v>
       </c>
       <c r="F13" s="35">
-        <f>C13/SUM($B13:$C13)</f>
+        <f t="shared" si="1"/>
         <v>0.35310024618288965</v>
       </c>
       <c r="G13" s="33">
@@ -6818,50 +6851,50 @@
         <v>30060</v>
       </c>
       <c r="I13" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>98614</v>
       </c>
       <c r="J13" s="40">
-        <f>G13/SUM($G13:$H13)</f>
+        <f t="shared" si="2"/>
         <v>0.69517512726387731</v>
       </c>
       <c r="K13" s="36">
-        <f>H13/SUM($G13:$H13)</f>
+        <f t="shared" si="3"/>
         <v>0.30482487273612269</v>
       </c>
       <c r="L13" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17839</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2378</v>
       </c>
       <c r="N13" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.35174997535245983</v>
       </c>
       <c r="O13" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8.59041976735785E-2</v>
       </c>
       <c r="P13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.8275373446766912E-2</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-4.8275373446766967E-2</v>
       </c>
       <c r="R13" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.2578797658073651</v>
       </c>
       <c r="S13" s="31">
         <v>67012</v>
       </c>
       <c r="T13" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1542</v>
       </c>
     </row>
@@ -6876,15 +6909,15 @@
         <v>1634</v>
       </c>
       <c r="D14" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8953</v>
       </c>
       <c r="E14" s="39">
-        <f>B14/SUM($B14:$C14)</f>
+        <f t="shared" si="0"/>
         <v>0.81749134368368148</v>
       </c>
       <c r="F14" s="35">
-        <f>C14/SUM($B14:$C14)</f>
+        <f t="shared" si="1"/>
         <v>0.18250865631631855</v>
       </c>
       <c r="G14" s="33">
@@ -6894,50 +6927,50 @@
         <v>1223</v>
       </c>
       <c r="I14" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>10170</v>
       </c>
       <c r="J14" s="40">
-        <f>G14/SUM($G14:$H14)</f>
+        <f t="shared" si="2"/>
         <v>0.87974434611602759</v>
       </c>
       <c r="K14" s="36">
-        <f>H14/SUM($G14:$H14)</f>
+        <f t="shared" si="3"/>
         <v>0.12025565388397247</v>
       </c>
       <c r="L14" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1628</v>
       </c>
       <c r="M14" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-411</v>
       </c>
       <c r="N14" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.222434758846837</v>
       </c>
       <c r="O14" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.25152998776009794</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6.2253002432346105E-2</v>
       </c>
       <c r="Q14" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-6.2253002432346077E-2</v>
       </c>
       <c r="R14" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.1359320898023009</v>
       </c>
       <c r="S14" s="31">
         <v>12744</v>
       </c>
       <c r="T14" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-3797</v>
       </c>
     </row>
@@ -6952,15 +6985,15 @@
         <v>19814</v>
       </c>
       <c r="D15" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>89800</v>
       </c>
       <c r="E15" s="39">
-        <f>B15/SUM($B15:$C15)</f>
+        <f t="shared" si="0"/>
         <v>0.77935412026726059</v>
       </c>
       <c r="F15" s="35">
-        <f>C15/SUM($B15:$C15)</f>
+        <f t="shared" si="1"/>
         <v>0.22064587973273941</v>
       </c>
       <c r="G15" s="33">
@@ -6970,50 +7003,50 @@
         <v>22560</v>
       </c>
       <c r="I15" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>105020</v>
       </c>
       <c r="J15" s="40">
-        <f>G15/SUM($G15:$H15)</f>
+        <f t="shared" si="2"/>
         <v>0.78518377451913923</v>
       </c>
       <c r="K15" s="36">
-        <f>H15/SUM($G15:$H15)</f>
+        <f t="shared" si="3"/>
         <v>0.2148162254808608</v>
       </c>
       <c r="L15" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>12474</v>
       </c>
       <c r="M15" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2746</v>
       </c>
       <c r="N15" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.17823564712942588</v>
       </c>
       <c r="O15" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.13858887655193297</v>
       </c>
       <c r="P15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5.8296542518786465E-3</v>
       </c>
       <c r="Q15" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-5.8296542518786187E-3</v>
       </c>
       <c r="R15" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.16948775055679288</v>
       </c>
       <c r="S15" s="31">
         <v>77772</v>
       </c>
       <c r="T15" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>4688</v>
       </c>
     </row>
@@ -7028,15 +7061,15 @@
         <v>49227</v>
       </c>
       <c r="D16" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>103580</v>
       </c>
       <c r="E16" s="39">
-        <f>B16/SUM($B16:$C16)</f>
+        <f t="shared" si="0"/>
         <v>0.52474415910407413</v>
       </c>
       <c r="F16" s="35">
-        <f>C16/SUM($B16:$C16)</f>
+        <f t="shared" si="1"/>
         <v>0.47525584089592587</v>
       </c>
       <c r="G16" s="33">
@@ -7046,50 +7079,50 @@
         <v>56734</v>
       </c>
       <c r="I16" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>133644</v>
       </c>
       <c r="J16" s="40">
-        <f>G16/SUM($G16:$H16)</f>
+        <f t="shared" si="2"/>
         <v>0.57548412199574994</v>
       </c>
       <c r="K16" s="36">
-        <f>H16/SUM($G16:$H16)</f>
+        <f t="shared" si="3"/>
         <v>0.42451587800425011</v>
       </c>
       <c r="L16" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>22557</v>
       </c>
       <c r="M16" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7507</v>
       </c>
       <c r="N16" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.41500929111548579</v>
       </c>
       <c r="O16" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.15249761309850285</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5.0739962891675816E-2</v>
       </c>
       <c r="Q16" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-5.0739962891675761E-2</v>
       </c>
       <c r="R16" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.29024908283452405</v>
       </c>
       <c r="S16" s="31">
         <v>55158</v>
       </c>
       <c r="T16" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>21752</v>
       </c>
     </row>
@@ -7104,15 +7137,15 @@
         <v>2603</v>
       </c>
       <c r="D17" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7612</v>
       </c>
       <c r="E17" s="39">
-        <f>B17/SUM($B17:$C17)</f>
+        <f t="shared" si="0"/>
         <v>0.65803993694167107</v>
       </c>
       <c r="F17" s="35">
-        <f>C17/SUM($B17:$C17)</f>
+        <f t="shared" si="1"/>
         <v>0.34196006305832893</v>
       </c>
       <c r="G17" s="33">
@@ -7122,50 +7155,50 @@
         <v>2059</v>
       </c>
       <c r="I17" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8123</v>
       </c>
       <c r="J17" s="40">
-        <f>G17/SUM($G17:$H17)</f>
+        <f t="shared" si="2"/>
         <v>0.74652222085436415</v>
       </c>
       <c r="K17" s="36">
-        <f>H17/SUM($G17:$H17)</f>
+        <f t="shared" si="3"/>
         <v>0.25347777914563585</v>
       </c>
       <c r="L17" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1055</v>
       </c>
       <c r="M17" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-544</v>
       </c>
       <c r="N17" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.21062088241165902</v>
       </c>
       <c r="O17" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.20898962735305418</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8.8482283912693083E-2</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-8.8482283912693083E-2</v>
       </c>
       <c r="R17" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6.7130846032580141E-2</v>
       </c>
       <c r="S17" s="31">
         <v>4786</v>
       </c>
       <c r="T17" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1278</v>
       </c>
     </row>
@@ -7180,15 +7213,15 @@
         <v>163694</v>
       </c>
       <c r="D18" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>261006</v>
       </c>
       <c r="E18" s="44">
-        <f>B18/SUM($B18:$C18)</f>
+        <f t="shared" si="0"/>
         <v>0.37283434097300444</v>
       </c>
       <c r="F18" s="44">
-        <f>C18/SUM($B18:$C18)</f>
+        <f t="shared" si="1"/>
         <v>0.6271656590269955</v>
       </c>
       <c r="G18" s="45">
@@ -7198,50 +7231,50 @@
         <v>193887</v>
       </c>
       <c r="I18" s="45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>352460</v>
       </c>
       <c r="J18" s="46">
-        <f>G18/SUM($G18:$H18)</f>
+        <f t="shared" si="2"/>
         <v>0.44990353515292514</v>
       </c>
       <c r="K18" s="46">
-        <f>H18/SUM($G18:$H18)</f>
+        <f t="shared" si="3"/>
         <v>0.55009646484707486</v>
       </c>
       <c r="L18" s="47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>61261</v>
       </c>
       <c r="M18" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>30193</v>
       </c>
       <c r="N18" s="46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.62953181519237089</v>
       </c>
       <c r="O18" s="46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.18444781115984704</v>
       </c>
       <c r="P18" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7.7069194179920697E-2</v>
       </c>
       <c r="Q18" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-7.7069194179920641E-2</v>
       </c>
       <c r="R18" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.35039041248093916</v>
       </c>
       <c r="S18" s="47">
         <v>112995</v>
       </c>
       <c r="T18" s="47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>45578</v>
       </c>
     </row>
@@ -7256,15 +7289,15 @@
         <v>184950</v>
       </c>
       <c r="D19" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>217569</v>
       </c>
       <c r="E19" s="44">
-        <f>B19/SUM($B19:$C19)</f>
+        <f t="shared" si="0"/>
         <v>0.14992485142644402</v>
       </c>
       <c r="F19" s="44">
-        <f>C19/SUM($B19:$C19)</f>
+        <f t="shared" si="1"/>
         <v>0.85007514857355593</v>
       </c>
       <c r="G19" s="45">
@@ -7274,50 +7307,50 @@
         <v>209485</v>
       </c>
       <c r="I19" s="45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>293080</v>
       </c>
       <c r="J19" s="46">
-        <f>G19/SUM($G19:$H19)</f>
+        <f t="shared" si="2"/>
         <v>0.2852292889313498</v>
       </c>
       <c r="K19" s="46">
-        <f>H19/SUM($G19:$H19)</f>
+        <f t="shared" si="3"/>
         <v>0.7147707110686502</v>
       </c>
       <c r="L19" s="47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>50976</v>
       </c>
       <c r="M19" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>24535</v>
       </c>
       <c r="N19" s="46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.5627701646279775</v>
       </c>
       <c r="O19" s="46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.1326574749932414</v>
       </c>
       <c r="P19" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.13530443750490578</v>
       </c>
       <c r="Q19" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-0.13530443750490573</v>
       </c>
       <c r="R19" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.34706690750980151</v>
       </c>
       <c r="S19" s="47">
         <v>40500</v>
       </c>
       <c r="T19" s="47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>43095</v>
       </c>
     </row>
@@ -7332,15 +7365,15 @@
         <v>3757</v>
       </c>
       <c r="D20" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>19193</v>
       </c>
       <c r="E20" s="39">
-        <f>B20/SUM($B20:$C20)</f>
+        <f t="shared" si="0"/>
         <v>0.80425155004428694</v>
       </c>
       <c r="F20" s="35">
-        <f>C20/SUM($B20:$C20)</f>
+        <f t="shared" si="1"/>
         <v>0.19574844995571303</v>
       </c>
       <c r="G20" s="33">
@@ -7350,50 +7383,50 @@
         <v>3019</v>
       </c>
       <c r="I20" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>21737</v>
       </c>
       <c r="J20" s="40">
-        <f>G20/SUM($G20:$H20)</f>
+        <f t="shared" si="2"/>
         <v>0.86111238901412335</v>
       </c>
       <c r="K20" s="36">
-        <f>H20/SUM($G20:$H20)</f>
+        <f t="shared" si="3"/>
         <v>0.13888761098587663</v>
       </c>
       <c r="L20" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3282</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-738</v>
       </c>
       <c r="N20" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.21261984970199532</v>
       </c>
       <c r="O20" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.19643332446100611</v>
       </c>
       <c r="P20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5.6860838969836403E-2</v>
       </c>
       <c r="Q20" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-5.6860838969836403E-2</v>
       </c>
       <c r="R20" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.13254832491012347</v>
       </c>
       <c r="S20" s="31">
         <v>17896</v>
       </c>
       <c r="T20" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>822</v>
       </c>
     </row>
@@ -7408,15 +7441,15 @@
         <v>8203</v>
       </c>
       <c r="D21" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>31878</v>
       </c>
       <c r="E21" s="39">
-        <f>B21/SUM($B21:$C21)</f>
+        <f t="shared" si="0"/>
         <v>0.74267519919693836</v>
       </c>
       <c r="F21" s="35">
-        <f>C21/SUM($B21:$C21)</f>
+        <f t="shared" si="1"/>
         <v>0.25732480080306169</v>
       </c>
       <c r="G21" s="33">
@@ -7426,50 +7459,50 @@
         <v>8253</v>
       </c>
       <c r="I21" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>37440</v>
       </c>
       <c r="J21" s="40">
-        <f>G21/SUM($G21:$H21)</f>
+        <f t="shared" si="2"/>
         <v>0.77956730769230764</v>
       </c>
       <c r="K21" s="36">
-        <f>H21/SUM($G21:$H21)</f>
+        <f t="shared" si="3"/>
         <v>0.2204326923076923</v>
       </c>
       <c r="L21" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5512</v>
       </c>
       <c r="M21" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="N21" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.2328194297782471</v>
       </c>
       <c r="O21" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.0953309764720225E-3</v>
       </c>
       <c r="P21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.689210849536928E-2</v>
       </c>
       <c r="Q21" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.6892108495369391E-2</v>
       </c>
       <c r="R21" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.17447769621682666</v>
       </c>
       <c r="S21" s="31">
         <v>29453</v>
       </c>
       <c r="T21" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-266</v>
       </c>
     </row>
@@ -7484,15 +7517,15 @@
         <v>2135</v>
       </c>
       <c r="D22" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6623</v>
       </c>
       <c r="E22" s="39">
-        <f>B22/SUM($B22:$C22)</f>
+        <f t="shared" si="0"/>
         <v>0.67763853238713578</v>
       </c>
       <c r="F22" s="35">
-        <f>C22/SUM($B22:$C22)</f>
+        <f t="shared" si="1"/>
         <v>0.32236146761286427</v>
       </c>
       <c r="G22" s="33">
@@ -7502,50 +7535,50 @@
         <v>1984</v>
       </c>
       <c r="I22" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6907</v>
       </c>
       <c r="J22" s="40">
-        <f>G22/SUM($G22:$H22)</f>
+        <f t="shared" si="2"/>
         <v>0.71275517590849857</v>
       </c>
       <c r="K22" s="36">
-        <f>H22/SUM($G22:$H22)</f>
+        <f t="shared" si="3"/>
         <v>0.28724482409150137</v>
       </c>
       <c r="L22" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>435</v>
       </c>
       <c r="M22" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-151</v>
       </c>
       <c r="N22" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>9.6925133689839571E-2</v>
       </c>
       <c r="O22" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-7.0725995316159251E-2</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.5116643521362789E-2</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.51166435213629E-2</v>
       </c>
       <c r="R22" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.2880869696512156E-2</v>
       </c>
       <c r="S22" s="31">
         <v>5301</v>
       </c>
       <c r="T22" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-378</v>
       </c>
     </row>
@@ -7560,15 +7593,15 @@
         <v>4420</v>
       </c>
       <c r="D23" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15036</v>
       </c>
       <c r="E23" s="39">
-        <f>B23/SUM($B23:$C23)</f>
+        <f t="shared" si="0"/>
         <v>0.70603884011705242</v>
       </c>
       <c r="F23" s="35">
-        <f>C23/SUM($B23:$C23)</f>
+        <f t="shared" si="1"/>
         <v>0.29396115988294758</v>
       </c>
       <c r="G23" s="33">
@@ -7578,50 +7611,50 @@
         <v>3637</v>
       </c>
       <c r="I23" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>16993</v>
       </c>
       <c r="J23" s="40">
-        <f>G23/SUM($G23:$H23)</f>
+        <f t="shared" si="2"/>
         <v>0.78597069381510032</v>
       </c>
       <c r="K23" s="36">
-        <f>H23/SUM($G23:$H23)</f>
+        <f t="shared" si="3"/>
         <v>0.21402930618489965</v>
       </c>
       <c r="L23" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2740</v>
       </c>
       <c r="M23" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-783</v>
       </c>
       <c r="N23" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.25810097965335344</v>
       </c>
       <c r="O23" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-0.17714932126696833</v>
       </c>
       <c r="P23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7.9931853698047894E-2</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-7.9931853698047922E-2</v>
       </c>
       <c r="R23" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.13015429635541367</v>
       </c>
       <c r="S23" s="31">
         <v>11535</v>
       </c>
       <c r="T23" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1821</v>
       </c>
     </row>
@@ -7636,15 +7669,15 @@
         <v>9661</v>
       </c>
       <c r="D24" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>38130</v>
       </c>
       <c r="E24" s="39">
-        <f>B24/SUM($B24:$C24)</f>
+        <f t="shared" si="0"/>
         <v>0.7466299501704694</v>
       </c>
       <c r="F24" s="35">
-        <f>C24/SUM($B24:$C24)</f>
+        <f t="shared" si="1"/>
         <v>0.25337004982953054</v>
       </c>
       <c r="G24" s="33">
@@ -7654,50 +7687,50 @@
         <v>9611</v>
       </c>
       <c r="I24" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>46225</v>
       </c>
       <c r="J24" s="40">
-        <f>G24/SUM($G24:$H24)</f>
+        <f t="shared" si="2"/>
         <v>0.7920822065981612</v>
       </c>
       <c r="K24" s="36">
-        <f>H24/SUM($G24:$H24)</f>
+        <f t="shared" si="3"/>
         <v>0.20791779340183883</v>
       </c>
       <c r="L24" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8145</v>
       </c>
       <c r="M24" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-50</v>
       </c>
       <c r="N24" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.28610067090519514</v>
       </c>
       <c r="O24" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-5.1754476762239932E-3</v>
       </c>
       <c r="P24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.5452256427691795E-2</v>
       </c>
       <c r="Q24" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-4.5452256427691712E-2</v>
       </c>
       <c r="R24" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.21230002622606872</v>
       </c>
       <c r="S24" s="31">
         <v>42395</v>
       </c>
       <c r="T24" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-5781</v>
       </c>
     </row>
@@ -7712,15 +7745,15 @@
         <v>8833</v>
       </c>
       <c r="D25" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>25502</v>
       </c>
       <c r="E25" s="39">
-        <f>B25/SUM($B25:$C25)</f>
+        <f t="shared" si="0"/>
         <v>0.65363500901890048</v>
       </c>
       <c r="F25" s="35">
-        <f>C25/SUM($B25:$C25)</f>
+        <f t="shared" si="1"/>
         <v>0.34636499098109952</v>
       </c>
       <c r="G25" s="33">
@@ -7730,50 +7763,50 @@
         <v>9576</v>
       </c>
       <c r="I25" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>31002</v>
       </c>
       <c r="J25" s="40">
-        <f>G25/SUM($G25:$H25)</f>
+        <f t="shared" si="2"/>
         <v>0.6911167021482485</v>
       </c>
       <c r="K25" s="36">
-        <f>H25/SUM($G25:$H25)</f>
+        <f t="shared" si="3"/>
         <v>0.3088832978517515</v>
       </c>
       <c r="L25" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4757</v>
       </c>
       <c r="M25" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>743</v>
       </c>
       <c r="N25" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.28538004679344892</v>
       </c>
       <c r="O25" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8.4116381750254723E-2</v>
       </c>
       <c r="P25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.7481693129348015E-2</v>
       </c>
       <c r="Q25" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.7481693129348015E-2</v>
       </c>
       <c r="R25" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.21566935926593991</v>
       </c>
       <c r="S25" s="31">
         <v>22811</v>
       </c>
       <c r="T25" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-1385</v>
       </c>
     </row>
@@ -7788,15 +7821,15 @@
         <v>5521</v>
       </c>
       <c r="D26" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18792</v>
       </c>
       <c r="E26" s="39">
-        <f>B26/SUM($B26:$C26)</f>
+        <f t="shared" si="0"/>
         <v>0.70620476798637721</v>
       </c>
       <c r="F26" s="35">
-        <f>C26/SUM($B26:$C26)</f>
+        <f t="shared" si="1"/>
         <v>0.29379523201362284</v>
       </c>
       <c r="G26" s="33">
@@ -7806,50 +7839,50 @@
         <v>5049</v>
       </c>
       <c r="I26" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>21974</v>
       </c>
       <c r="J26" s="40">
-        <f>G26/SUM($G26:$H26)</f>
+        <f t="shared" si="2"/>
         <v>0.77022845180668065</v>
       </c>
       <c r="K26" s="36">
-        <f>H26/SUM($G26:$H26)</f>
+        <f t="shared" si="3"/>
         <v>0.22977154819331938</v>
       </c>
       <c r="L26" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3654</v>
       </c>
       <c r="M26" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-472</v>
       </c>
       <c r="N26" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.27533720141662271</v>
       </c>
       <c r="O26" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-8.5491758739358811E-2</v>
       </c>
       <c r="P26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6.4023683820303434E-2</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-6.4023683820303462E-2</v>
       </c>
       <c r="R26" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.16932737335036185</v>
       </c>
       <c r="S26" s="31">
         <v>17088</v>
       </c>
       <c r="T26" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-163</v>
       </c>
     </row>
@@ -8064,4 +8097,1372 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1980C6B1-A5A7-FC41-8F62-100936BC21AE}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="55">
+        <v>15410</v>
+      </c>
+      <c r="C2">
+        <v>20478</v>
+      </c>
+      <c r="D2" s="36">
+        <f>B2/C2</f>
+        <v>0.7525148940326204</v>
+      </c>
+      <c r="E2" s="33">
+        <v>18048</v>
+      </c>
+      <c r="F2">
+        <v>21533</v>
+      </c>
+      <c r="G2" s="36">
+        <f>E2/F2</f>
+        <v>0.83815538940231271</v>
+      </c>
+      <c r="H2" s="4">
+        <f>G2-D2</f>
+        <v>8.5640495369692315E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="55">
+        <v>119195</v>
+      </c>
+      <c r="C3">
+        <v>180338</v>
+      </c>
+      <c r="D3" s="36">
+        <f t="shared" ref="D3:D25" si="0">B3/C3</f>
+        <v>0.66095332098614823</v>
+      </c>
+      <c r="E3" s="57">
+        <v>147985</v>
+      </c>
+      <c r="F3">
+        <v>213711</v>
+      </c>
+      <c r="G3" s="36">
+        <f t="shared" ref="G3:G25" si="1">E3/F3</f>
+        <v>0.69245382783291454</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H25" si="2">G3-D3</f>
+        <v>3.1500506846766307E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="55">
+        <v>30845</v>
+      </c>
+      <c r="C4">
+        <v>140686</v>
+      </c>
+      <c r="D4" s="36">
+        <f t="shared" si="0"/>
+        <v>0.21924711769472441</v>
+      </c>
+      <c r="E4" s="57">
+        <v>54136</v>
+      </c>
+      <c r="F4">
+        <v>169750</v>
+      </c>
+      <c r="G4" s="36">
+        <f t="shared" si="1"/>
+        <v>0.31891605301914583</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="2"/>
+        <v>9.966893532442142E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="55">
+        <v>155936</v>
+      </c>
+      <c r="C5">
+        <v>264143</v>
+      </c>
+      <c r="D5" s="36">
+        <f t="shared" si="0"/>
+        <v>0.59034689543164121</v>
+      </c>
+      <c r="E5" s="57">
+        <v>188110</v>
+      </c>
+      <c r="F5">
+        <v>304808</v>
+      </c>
+      <c r="G5" s="36">
+        <f t="shared" si="1"/>
+        <v>0.61714259468255428</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="2"/>
+        <v>2.6795699250913074E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="55">
+        <v>22739</v>
+      </c>
+      <c r="C6">
+        <v>32904</v>
+      </c>
+      <c r="D6" s="36">
+        <f t="shared" si="0"/>
+        <v>0.6910709944079747</v>
+      </c>
+      <c r="E6" s="57">
+        <v>28099</v>
+      </c>
+      <c r="F6">
+        <v>36985</v>
+      </c>
+      <c r="G6" s="36">
+        <f t="shared" si="1"/>
+        <v>0.75974043531161284</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="2"/>
+        <v>6.8669440903638135E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="55">
+        <v>7144</v>
+      </c>
+      <c r="C7">
+        <v>9208</v>
+      </c>
+      <c r="D7" s="36">
+        <f t="shared" si="0"/>
+        <v>0.77584708948740222</v>
+      </c>
+      <c r="E7" s="64">
+        <v>9166</v>
+      </c>
+      <c r="F7">
+        <v>11071</v>
+      </c>
+      <c r="G7" s="36">
+        <f t="shared" si="1"/>
+        <v>0.82792882305121485</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="2"/>
+        <v>5.2081733563812627E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="55">
+        <v>52951</v>
+      </c>
+      <c r="C8">
+        <v>64419</v>
+      </c>
+      <c r="D8" s="36">
+        <f t="shared" si="0"/>
+        <v>0.82197798786072429</v>
+      </c>
+      <c r="E8" s="57">
+        <v>60214</v>
+      </c>
+      <c r="F8">
+        <v>71847</v>
+      </c>
+      <c r="G8" s="36">
+        <f t="shared" si="1"/>
+        <v>0.83808648934541452</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="2"/>
+        <v>1.610850148469023E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="55">
+        <v>20699</v>
+      </c>
+      <c r="C9">
+        <v>26766</v>
+      </c>
+      <c r="D9" s="36">
+        <f t="shared" si="0"/>
+        <v>0.77333183890009716</v>
+      </c>
+      <c r="E9" s="57">
+        <v>26171</v>
+      </c>
+      <c r="F9">
+        <v>33575</v>
+      </c>
+      <c r="G9" s="36">
+        <f t="shared" si="1"/>
+        <v>0.77947877885331351</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="2"/>
+        <v>6.1469399532163571E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="55">
+        <v>22268</v>
+      </c>
+      <c r="C10">
+        <v>47469</v>
+      </c>
+      <c r="D10" s="36">
+        <f t="shared" si="0"/>
+        <v>0.46910615348964585</v>
+      </c>
+      <c r="E10" s="57">
+        <v>30294</v>
+      </c>
+      <c r="F10">
+        <v>61030</v>
+      </c>
+      <c r="G10" s="36">
+        <f t="shared" si="1"/>
+        <v>0.49637883008356548</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="2"/>
+        <v>2.7272676593919631E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="55">
+        <v>7276</v>
+      </c>
+      <c r="C11">
+        <v>10660</v>
+      </c>
+      <c r="D11" s="36">
+        <f t="shared" si="0"/>
+        <v>0.68255159474671667</v>
+      </c>
+      <c r="E11" s="57">
+        <v>8721</v>
+      </c>
+      <c r="F11">
+        <v>11672</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" si="1"/>
+        <v>0.74717272104180943</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="2"/>
+        <v>6.4621126295092757E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="55">
+        <v>50715</v>
+      </c>
+      <c r="C12">
+        <v>80072</v>
+      </c>
+      <c r="D12" s="36">
+        <f t="shared" si="0"/>
+        <v>0.63336746927765009</v>
+      </c>
+      <c r="E12" s="57">
+        <v>68554</v>
+      </c>
+      <c r="F12">
+        <v>99807</v>
+      </c>
+      <c r="G12" s="36">
+        <f t="shared" si="1"/>
+        <v>0.68686565070586236</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="2"/>
+        <v>5.3498181428212277E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="55">
+        <v>7319</v>
+      </c>
+      <c r="C13">
+        <v>9182</v>
+      </c>
+      <c r="D13" s="36">
+        <f t="shared" si="0"/>
+        <v>0.7971030276628186</v>
+      </c>
+      <c r="E13" s="57">
+        <v>8947</v>
+      </c>
+      <c r="F13">
+        <v>10304</v>
+      </c>
+      <c r="G13" s="36">
+        <f t="shared" si="1"/>
+        <v>0.8683035714285714</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="2"/>
+        <v>7.12005437657528E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="55">
+        <v>69986</v>
+      </c>
+      <c r="C14">
+        <f>19814+69986+1422+3+235</f>
+        <v>91460</v>
+      </c>
+      <c r="D14" s="36">
+        <f t="shared" si="0"/>
+        <v>0.76520883446315324</v>
+      </c>
+      <c r="E14" s="57">
+        <v>82460</v>
+      </c>
+      <c r="F14">
+        <v>106245</v>
+      </c>
+      <c r="G14" s="36">
+        <f t="shared" si="1"/>
+        <v>0.77613064144195021</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="2"/>
+        <v>1.0921806978796966E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="55">
+        <v>54353</v>
+      </c>
+      <c r="C15">
+        <f>49227+54353+1575+12+2+284</f>
+        <v>105453</v>
+      </c>
+      <c r="D15" s="36">
+        <f t="shared" si="0"/>
+        <v>0.51542393293694821</v>
+      </c>
+      <c r="E15" s="57">
+        <v>76910</v>
+      </c>
+      <c r="F15">
+        <v>135176</v>
+      </c>
+      <c r="G15" s="36">
+        <f t="shared" si="1"/>
+        <v>0.56896194590755755</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="2"/>
+        <v>5.3538012970609339E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="55">
+        <v>5009</v>
+      </c>
+      <c r="C16">
+        <f>2603+5009+113+1+30</f>
+        <v>7756</v>
+      </c>
+      <c r="D16" s="36">
+        <f t="shared" si="0"/>
+        <v>0.64582258896338318</v>
+      </c>
+      <c r="E16" s="57">
+        <v>6064</v>
+      </c>
+      <c r="F16">
+        <v>8220</v>
+      </c>
+      <c r="G16" s="36">
+        <f t="shared" si="1"/>
+        <v>0.73771289537712892</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="2"/>
+        <v>9.1890306413745737E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="55">
+        <v>97312</v>
+      </c>
+      <c r="C17">
+        <f>163694+97312+3286+9+518</f>
+        <v>264819</v>
+      </c>
+      <c r="D17" s="36">
+        <f t="shared" si="0"/>
+        <v>0.36746608060599883</v>
+      </c>
+      <c r="E17" s="57">
+        <v>158573</v>
+      </c>
+      <c r="F17">
+        <v>356202</v>
+      </c>
+      <c r="G17" s="36">
+        <f t="shared" si="1"/>
+        <v>0.44517717474915919</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="2"/>
+        <v>7.7711094143160353E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="55">
+        <v>32619</v>
+      </c>
+      <c r="C18">
+        <f>184950+32619+1711+13+279</f>
+        <v>219572</v>
+      </c>
+      <c r="D18" s="36">
+        <f t="shared" si="0"/>
+        <v>0.14855719308472848</v>
+      </c>
+      <c r="E18" s="57">
+        <v>83595</v>
+      </c>
+      <c r="F18">
+        <v>295982</v>
+      </c>
+      <c r="G18" s="36">
+        <f t="shared" si="1"/>
+        <v>0.28243271550296978</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1338755224182413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="55">
+        <v>15436</v>
+      </c>
+      <c r="C19">
+        <f>3757+15436+197+8+28</f>
+        <v>19426</v>
+      </c>
+      <c r="D19" s="36">
+        <f t="shared" si="0"/>
+        <v>0.79460516833110262</v>
+      </c>
+      <c r="E19" s="57">
+        <v>18718</v>
+      </c>
+      <c r="F19">
+        <v>21924</v>
+      </c>
+      <c r="G19" s="36">
+        <f t="shared" si="1"/>
+        <v>0.85376756066411241</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="2"/>
+        <v>5.9162392333009794E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="55">
+        <v>23675</v>
+      </c>
+      <c r="C20">
+        <f>8203+23675+645+34</f>
+        <v>32557</v>
+      </c>
+      <c r="D20" s="36">
+        <f t="shared" si="0"/>
+        <v>0.72718616580151729</v>
+      </c>
+      <c r="E20" s="57">
+        <v>29187</v>
+      </c>
+      <c r="F20">
+        <v>37993</v>
+      </c>
+      <c r="G20" s="36">
+        <f t="shared" si="1"/>
+        <v>0.76822046166399072</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="2"/>
+        <v>4.1034295862473424E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="55">
+        <v>4488</v>
+      </c>
+      <c r="C21">
+        <f>2135+4488+77+1</f>
+        <v>6701</v>
+      </c>
+      <c r="D21" s="36">
+        <f t="shared" si="0"/>
+        <v>0.66975078346515449</v>
+      </c>
+      <c r="E21" s="57">
+        <v>4923</v>
+      </c>
+      <c r="F21">
+        <v>7015</v>
+      </c>
+      <c r="G21" s="36">
+        <f t="shared" si="1"/>
+        <v>0.70178189593727724</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="2"/>
+        <v>3.2031112472122758E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="55">
+        <v>10616</v>
+      </c>
+      <c r="C22">
+        <f>4420+10616+168+22</f>
+        <v>15226</v>
+      </c>
+      <c r="D22" s="36">
+        <f t="shared" si="0"/>
+        <v>0.69722842506239324</v>
+      </c>
+      <c r="E22" s="57">
+        <v>13356</v>
+      </c>
+      <c r="F22">
+        <v>17135</v>
+      </c>
+      <c r="G22" s="36">
+        <f t="shared" si="1"/>
+        <v>0.77945725124015175</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="2"/>
+        <v>8.2228826177758507E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="55">
+        <v>28469</v>
+      </c>
+      <c r="C23">
+        <f>9661+28469+653+6+32</f>
+        <v>38821</v>
+      </c>
+      <c r="D23" s="36">
+        <f t="shared" si="0"/>
+        <v>0.73334020246773657</v>
+      </c>
+      <c r="E23" s="57">
+        <v>36614</v>
+      </c>
+      <c r="F23">
+        <v>46946</v>
+      </c>
+      <c r="G23" s="36">
+        <f t="shared" si="1"/>
+        <v>0.77991735185106292</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="2"/>
+        <v>4.6577149383326355E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="55">
+        <v>16669</v>
+      </c>
+      <c r="C24">
+        <f>8833+16669+396+26</f>
+        <v>25924</v>
+      </c>
+      <c r="D24" s="36">
+        <f t="shared" si="0"/>
+        <v>0.64299490819318006</v>
+      </c>
+      <c r="E24" s="33">
+        <v>21426</v>
+      </c>
+      <c r="F24">
+        <v>31410</v>
+      </c>
+      <c r="G24" s="36">
+        <f t="shared" si="1"/>
+        <v>0.68213944603629417</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="2"/>
+        <v>3.9144537843114113E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="55">
+        <v>13271</v>
+      </c>
+      <c r="C25">
+        <f>5521+13271+331+14</f>
+        <v>19137</v>
+      </c>
+      <c r="D25" s="36">
+        <f t="shared" si="0"/>
+        <v>0.69347337618226468</v>
+      </c>
+      <c r="E25" s="33">
+        <v>16925</v>
+      </c>
+      <c r="F25">
+        <v>22196</v>
+      </c>
+      <c r="G25" s="36">
+        <f t="shared" si="1"/>
+        <v>0.76252477923950257</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="2"/>
+        <v>6.9051403057237892E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8CE833-6403-2448-92BE-0DD088BF40B2}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <f>184950+32619+1711+13+279</f>
+        <v>219572</v>
+      </c>
+      <c r="C2">
+        <v>295982</v>
+      </c>
+      <c r="D2" s="65">
+        <f>((C2-B2)/B2)*100</f>
+        <v>34.799519064361576</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <f>163694+97312+3286+9+518</f>
+        <v>264819</v>
+      </c>
+      <c r="C3">
+        <v>356202</v>
+      </c>
+      <c r="D3" s="65">
+        <f>((C3-B3)/B3)*100</f>
+        <v>34.50772036749629</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>47469</v>
+      </c>
+      <c r="C4">
+        <v>61030</v>
+      </c>
+      <c r="D4" s="65">
+        <f>((C4-B4)/B4)*100</f>
+        <v>28.568118140259958</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <f>49227+54353+1575+12+2+284</f>
+        <v>105453</v>
+      </c>
+      <c r="C5">
+        <v>135176</v>
+      </c>
+      <c r="D5" s="65">
+        <f>((C5-B5)/B5)*100</f>
+        <v>28.186016519207609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>26766</v>
+      </c>
+      <c r="C6">
+        <v>33575</v>
+      </c>
+      <c r="D6" s="65">
+        <f>((C6-B6)/B6)*100</f>
+        <v>25.43898976313233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>80072</v>
+      </c>
+      <c r="C7">
+        <v>99807</v>
+      </c>
+      <c r="D7" s="65">
+        <f>((C7-B7)/B7)*100</f>
+        <v>24.646568088720151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <f>8833+16669+396+26</f>
+        <v>25924</v>
+      </c>
+      <c r="C8">
+        <v>31410</v>
+      </c>
+      <c r="D8" s="65">
+        <f>((C8-B8)/B8)*100</f>
+        <v>21.161857738003395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <f>9661+28469+653+6+32</f>
+        <v>38821</v>
+      </c>
+      <c r="C9">
+        <v>46946</v>
+      </c>
+      <c r="D9" s="65">
+        <f>((C9-B9)/B9)*100</f>
+        <v>20.929393884753097</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>140686</v>
+      </c>
+      <c r="C10">
+        <v>169750</v>
+      </c>
+      <c r="D10" s="65">
+        <f>((C10-B10)/B10)*100</f>
+        <v>20.658772017116132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>9208</v>
+      </c>
+      <c r="C11">
+        <v>11071</v>
+      </c>
+      <c r="D11" s="65">
+        <f>((C11-B11)/B11)*100</f>
+        <v>20.232406602953954</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>180338</v>
+      </c>
+      <c r="C12">
+        <v>213711</v>
+      </c>
+      <c r="D12" s="65">
+        <f>((C12-B12)/B12)*100</f>
+        <v>18.505805764730674</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <f>8203+23675+645+34</f>
+        <v>32557</v>
+      </c>
+      <c r="C13">
+        <v>37993</v>
+      </c>
+      <c r="D13" s="65">
+        <f>((C13-B13)/B13)*100</f>
+        <v>16.696870104739382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <f>19814+69986+1422+3+235</f>
+        <v>91460</v>
+      </c>
+      <c r="C14">
+        <v>106245</v>
+      </c>
+      <c r="D14" s="65">
+        <f>((C14-B14)/B14)*100</f>
+        <v>16.165536846708946</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <f>5521+13271+331+14</f>
+        <v>19137</v>
+      </c>
+      <c r="C15">
+        <v>22196</v>
+      </c>
+      <c r="D15" s="65">
+        <f>((C15-B15)/B15)*100</f>
+        <v>15.984741600041804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>264143</v>
+      </c>
+      <c r="C16">
+        <v>304808</v>
+      </c>
+      <c r="D16" s="65">
+        <f>((C16-B16)/B16)*100</f>
+        <v>15.395070094607846</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <f>3757+15436+197+8+28</f>
+        <v>19426</v>
+      </c>
+      <c r="C17">
+        <v>21924</v>
+      </c>
+      <c r="D17" s="65">
+        <f>((C17-B17)/B17)*100</f>
+        <v>12.859054874909914</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <f>4420+10616+168+22</f>
+        <v>15226</v>
+      </c>
+      <c r="C18">
+        <v>17135</v>
+      </c>
+      <c r="D18" s="65">
+        <f>((C18-B18)/B18)*100</f>
+        <v>12.537764350453173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>32904</v>
+      </c>
+      <c r="C19">
+        <v>36985</v>
+      </c>
+      <c r="D19" s="65">
+        <f>((C19-B19)/B19)*100</f>
+        <v>12.402747386336008</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>9182</v>
+      </c>
+      <c r="C20">
+        <v>10304</v>
+      </c>
+      <c r="D20" s="65">
+        <f>((C20-B20)/B20)*100</f>
+        <v>12.219560008712699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>64419</v>
+      </c>
+      <c r="C21">
+        <v>71847</v>
+      </c>
+      <c r="D21" s="65">
+        <f>((C21-B21)/B21)*100</f>
+        <v>11.530759558515346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>10660</v>
+      </c>
+      <c r="C22">
+        <v>11672</v>
+      </c>
+      <c r="D22" s="65">
+        <f>((C22-B22)/B22)*100</f>
+        <v>9.4934333958724206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <f>2603+5009+113+1+30</f>
+        <v>7756</v>
+      </c>
+      <c r="C23">
+        <v>8220</v>
+      </c>
+      <c r="D23" s="65">
+        <f>((C23-B23)/B23)*100</f>
+        <v>5.9824651882413615</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>20478</v>
+      </c>
+      <c r="C24">
+        <v>21533</v>
+      </c>
+      <c r="D24" s="65">
+        <f>((C24-B24)/B24)*100</f>
+        <v>5.151870299833968</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <f>2135+4488+77+1</f>
+        <v>6701</v>
+      </c>
+      <c r="C25">
+        <v>7015</v>
+      </c>
+      <c r="D25" s="65">
+        <f>((C25-B25)/B25)*100</f>
+        <v>4.6858677809282199</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D25">
+    <sortCondition descending="1" ref="D1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D42AA58-2A10-2443-AFEF-0B7DF7E2AB0B}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="59">
+        <v>142739</v>
+      </c>
+      <c r="C2" s="57">
+        <v>45371</v>
+      </c>
+      <c r="D2" s="31"/>
+    </row>
+    <row r="3" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="59">
+        <v>112995</v>
+      </c>
+      <c r="C3" s="57">
+        <v>45578</v>
+      </c>
+      <c r="D3" s="31"/>
+    </row>
+    <row r="4" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="31">
+        <v>134806</v>
+      </c>
+      <c r="C4" s="33">
+        <v>13179</v>
+      </c>
+      <c r="D4" s="31"/>
+    </row>
+    <row r="5" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="59">
+        <v>40500</v>
+      </c>
+      <c r="C5" s="57">
+        <v>43095</v>
+      </c>
+      <c r="D5" s="31"/>
+    </row>
+    <row r="6" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="59">
+        <v>77772</v>
+      </c>
+      <c r="C6" s="57">
+        <v>4688</v>
+      </c>
+      <c r="D6" s="31"/>
+    </row>
+    <row r="7" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="59">
+        <v>55158</v>
+      </c>
+      <c r="C7" s="57">
+        <v>21752</v>
+      </c>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="59">
+        <v>67012</v>
+      </c>
+      <c r="C8" s="57">
+        <v>1542</v>
+      </c>
+      <c r="D8" s="31"/>
+    </row>
+    <row r="9" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="59">
+        <v>30873</v>
+      </c>
+      <c r="C9" s="57">
+        <v>23263</v>
+      </c>
+      <c r="D9" s="31"/>
+    </row>
+    <row r="10" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="59">
+        <v>24871</v>
+      </c>
+      <c r="C10" s="57">
+        <v>5423</v>
+      </c>
+      <c r="D10" s="31"/>
+    </row>
+    <row r="11" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="59">
+        <v>27415</v>
+      </c>
+      <c r="C11" s="57">
+        <v>684</v>
+      </c>
+      <c r="D11" s="31"/>
+    </row>
+    <row r="12" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="59">
+        <v>17896</v>
+      </c>
+      <c r="C12" s="57">
+        <v>822</v>
+      </c>
+      <c r="D12" s="31"/>
+    </row>
+    <row r="13" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="31">
+        <v>11535</v>
+      </c>
+      <c r="C13" s="33">
+        <v>1821</v>
+      </c>
+      <c r="D13" s="31"/>
+    </row>
+    <row r="14" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="59">
+        <v>8182</v>
+      </c>
+      <c r="C14" s="57">
+        <v>539</v>
+      </c>
+      <c r="D14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="59">
+        <v>4786</v>
+      </c>
+      <c r="C15" s="57">
+        <v>1278</v>
+      </c>
+      <c r="D15" s="31"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D15">
+    <sortCondition descending="1" ref="D1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>